<commit_message>
Dokumentation Algorithmus und Präsentation
</commit_message>
<xml_diff>
--- a/Dokumentation/Zeitplan.xlsx
+++ b/Dokumentation/Zeitplan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DH_Loerrach\2. Semester\Informatik\Projektarbeit\Entwicklung eines intelligenten Empfehlungssystems Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c18a77c3a83b4ea/Dokumente/Uni/PDF/Informatik/2_Semester_Projekt/Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035CE005-F14A-486F-9773-8288552C0D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{035CE005-F14A-486F-9773-8288552C0D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B659B96-FFC6-4B46-8AD3-DA94BD72331F}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="12900" xr2:uid="{89FA5042-C8BC-441E-88DF-91C29BA6D975}"/>
+    <workbookView xWindow="42300" yWindow="2505" windowWidth="28800" windowHeight="15345" xr2:uid="{89FA5042-C8BC-441E-88DF-91C29BA6D975}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -470,6 +470,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -515,14 +522,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -925,44 +924,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C9BBEE-C9E2-401A-AAB4-5A9F04353E65}">
   <dimension ref="A3:AM36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG35" sqref="AG35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:AE36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.46484375" customWidth="1"/>
-    <col min="2" max="2" width="14.53125" customWidth="1"/>
-    <col min="3" max="31" width="4.1328125" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="31" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -978,146 +977,146 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="31">
         <v>45797</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="31">
         <v>45825</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="15" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+    </row>
+    <row r="8" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A9" s="16"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A10" s="16"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A11" s="16"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A12" s="17"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="29" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29" t="s">
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29" t="s">
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="29"/>
-      <c r="AA13" s="29"/>
-      <c r="AB13" s="29"/>
-      <c r="AC13" s="29"/>
-      <c r="AD13" s="29" t="s">
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AE13" s="29"/>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="AE13" s="15"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1216,7 @@
       <c r="AL14" s="10"/>
       <c r="AM14" s="10"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
@@ -1257,7 +1256,7 @@
       <c r="AL15" s="13"/>
       <c r="AM15" s="13"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -1299,7 +1298,7 @@
       <c r="AL16" s="13"/>
       <c r="AM16" s="13"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1341,7 +1340,7 @@
       <c r="AL17" s="11"/>
       <c r="AM17" s="11"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
@@ -1383,7 +1382,7 @@
       <c r="AL18" s="11"/>
       <c r="AM18" s="11"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1424,7 @@
       <c r="AL19" s="11"/>
       <c r="AM19" s="11"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1467,7 +1466,7 @@
       <c r="AL20" s="11"/>
       <c r="AM20" s="11"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1504,7 +1503,7 @@
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
@@ -1539,7 +1538,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
@@ -1576,7 +1575,7 @@
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
@@ -1613,7 +1612,7 @@
       <c r="AD24" s="2"/>
       <c r="AE24" s="2"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -1650,7 +1649,7 @@
       <c r="AD25" s="2"/>
       <c r="AE25" s="2"/>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1687,7 +1686,7 @@
       <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1724,7 +1723,7 @@
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -1761,7 +1760,7 @@
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
@@ -1788,15 +1787,15 @@
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
-      <c r="Y29" s="30"/>
+      <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
-      <c r="AB29" s="30"/>
-      <c r="AC29" s="30"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
@@ -1813,7 +1812,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="30"/>
+      <c r="M30" s="2"/>
       <c r="N30" s="7"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
@@ -1833,7 +1832,7 @@
       <c r="AD30" s="7"/>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -1870,7 +1869,7 @@
       <c r="AD31" s="7"/>
       <c r="AE31" s="2"/>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>43</v>
       </c>
@@ -1892,7 +1891,7 @@
       <c r="Q32" s="7"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
-      <c r="T32" s="30"/>
+      <c r="T32" s="2"/>
       <c r="U32" s="7"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
@@ -1905,68 +1904,63 @@
       <c r="AD32" s="7"/>
       <c r="AE32" s="2"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A34" s="31" t="s">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
-      <c r="Q34" s="31"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="31"/>
-      <c r="T34" s="31"/>
-      <c r="U34" s="31"/>
-      <c r="V34" s="31"/>
-      <c r="W34" s="31"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="31"/>
-      <c r="Z34" s="31"/>
-      <c r="AA34" s="31"/>
-      <c r="AB34" s="31"/>
-      <c r="AC34" s="31"/>
-      <c r="AD34" s="31"/>
-      <c r="AE34" s="31"/>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="C36" s="32"/>
-      <c r="D36" s="31" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="16"/>
+      <c r="Y34" s="16"/>
+      <c r="Z34" s="16"/>
+      <c r="AA34" s="16"/>
+      <c r="AB34" s="16"/>
+      <c r="AC34" s="16"/>
+      <c r="AD34" s="16"/>
+      <c r="AE34" s="16"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C36" s="14"/>
+      <c r="D36" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
-      <c r="Q36" s="31"/>
-      <c r="R36" s="31"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="P13:V13"/>
-    <mergeCell ref="W13:AC13"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="A34:AE34"/>
-    <mergeCell ref="D36:R36"/>
     <mergeCell ref="A3:J4"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:J12"/>
@@ -1975,10 +1969,15 @@
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="C13:H13"/>
     <mergeCell ref="I13:O13"/>
+    <mergeCell ref="P13:V13"/>
+    <mergeCell ref="W13:AC13"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="A34:AE34"/>
+    <mergeCell ref="D36:R36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>